<commit_message>
update main.py, update readme, add note in instructions
</commit_message>
<xml_diff>
--- a/keyWords.xlsx
+++ b/keyWords.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yzh7ty\Documents\MS_SW\CIS-580\Project\project_main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D636722F-B864-4DFB-AC9E-E7C7A8B84264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD44213C-0E60-40F8-A6DC-1BF26F60D4FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29940" yWindow="3600" windowWidth="21600" windowHeight="10695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Sensor functions</t>
   </si>
@@ -450,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,7 +517,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -537,7 +537,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
@@ -551,7 +551,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
         <v>17</v>
@@ -565,7 +565,7 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
         <v>32</v>
@@ -579,7 +579,7 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
         <v>33</v>
@@ -587,11 +587,6 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>